<commit_message>
Subindo novas alterações de funcionamento
</commit_message>
<xml_diff>
--- a/Coletor-de-perifericos-Kabum/Perifericos_da_Kabum.xlsx
+++ b/Coletor-de-perifericos-Kabum/Perifericos_da_Kabum.xlsx
@@ -473,27 +473,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Teclado Com Fio, Mecânico Gamer Neologic Precision Pro Polar 60%, RGB, Hot Swap, 61 Teclas, Switch Red Branco, Cabo Tipo C - Proplr-red</t>
+          <t>Teclado Sem Fio Mecânico Gamer Logitech G PRO X 60 Lightspeed, RGB, Bluetooth, Compatível com Windows, Rosa Magenta - 920-011940</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/659446/Teclado-Gamer-Mec-nico-Neologic-Precision-Pro-Polar-60-RGB-Hot-Swap-61-Teclas-Switch-Red-Branco-Cabo-Tipo-C-Proplr-red_1730471401_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940_1718883113_m.jpg</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 219,99</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 199,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -505,27 +505,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Gamer Corsair K70 CORE RGB, Switch Corsair Red, Preto, BR - CH-910971E-BR</t>
+          <t>Teclado Gamer Logitech G PRO X TKL RAPID, Switches Magnético-analógicos, Modo Rapid Trigger, Layout US, Preto - 920-013131</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/508835/teclado-mecanico-gamer-corsair-k70-rgb-corsair-linear-red-preto-us-ch-910971e-br_1736944144_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/703012/teclado-gamer-logitech-g-pro-x-tkl-rapid-switches-magnetico-analogicos-modo-rapid-trigger-layout-us-preto-920-013131_1740581669_m.jpg</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 941,16</t>
+          <t>R$ 1.647,04</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 429,99</t>
+          <t>R$ 1.189,99</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -537,27 +537,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Teclado Gamer Mecanico Neologic Crystal Edge, 65%, Transparente, Rainbow, Switch Branco, Cabo Tipo C, Abnt2 - Nlcrstl-edge U Unica Unica</t>
+          <t>Teclado Gamer Logitech G213, RGB LIGHTSYNC, Controles de Mídia Dedicados, Design Durável Resistente à Respingos, ABNT2, Preto - 920-009438</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/623591/Teclado-Gamer-Mecanico-Neologic-Crystal-Edge-65-Transparente-Rainbow-Switch-Branco-Cabo-Tipo-C-Abnt2-Nlcrstl-edge_1725979232_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/107334/teclado-gamer-logitech-g213-prodigy-rgb-abnt2-920-009438_1613584305_m.jpg</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 259,00</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 219,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -569,27 +569,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Teclado Gamer Redragon Lakshmi, Switch Brown, Layout 60%, ABNT2, Branco - K606-YL&amp;GY&amp;WT (PT-BROWN)</t>
+          <t>Teclado Mecânico Gamer Logitech G G413 SE, USB, Anti-Ghosting, ABNT2, Preto - 920-010554</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/401373/teclado-gamer-redragon-lakshmi-switch-brown-layout-60-abnt2-branco-k606-yl-gy-wt-pt-brown-_1671623020_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/447929/teclado-mecanico-gamer-logitech-g-g413-se-usb-anti-ghosting-abnt2-preto-920-010554_1710951676_m.jpg</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 235,28</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 149,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -601,27 +601,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Teclado Semi-Mecânico Gamer Rise Mode G1, Rainbow, USB, Preto e Cinza - RM-TG-01-BG</t>
+          <t>Teclado Mecânico Gamer Sem Fio Logitech G715, Coleção Aurora, LIGHTSPEED Switch GX Red Linear, RGB, Layout ABNT, Apoio em Formato de Nuvem, Branco - 920-010706</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/588421/teclado-semi-mecanico-gamer-rise-mode-g1-rainbow-usb-preto-e-cinza-rm-tg-01-bg_1730978282_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/388064/teclado-mecanico-gamer-sem-fio-logitech-g715-rgb-led-bluetooth-usb-switch-gx-brown-linear-abnt-branco-920-010706_1665071178_m.jpg</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 82,34</t>
+          <t>R$ 1.647,05</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 34,99</t>
+          <t>R$ 1.139,99</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -633,27 +633,27 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Gamer Redragon Kumara, Anti-Ghosting, RGB, Switch Outemu Brown, ABNT2, Preto, PT - K552RGB-1 (PT-BROWN)</t>
+          <t>Teclado Mecânico Gamer Sem Fio Logitech G915 X Lightspeed, Design TKL RGB Lightsync, USB ou Bluetooth e Switch GL Tactile, Preto - 920-012715</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/93160/93160_1523969683_index_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/652581/teclado-mecanico-gamer-sem-fio-logitech-g915-x-lightspeed-design-tkl-rgb-lightsync-usb-ou-bluetooth-e-switch-gl-tactile-preto-920-012715_1731263951_m.jpg</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 282,34</t>
+          <t>R$ 1.333,32</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 199,99</t>
+          <t>R$ 1.099,99</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -665,27 +665,27 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Teclado Gamer Semi Mecânico Rise Mode G1 Full, USB, Branco - RM-TG-01-FW</t>
+          <t>Teclado Sem Fio Mecânico Gamer Logitech G PRO X 60 Lightspeed, RGB, Bluetooth, Compatível com Windows, Preto - 920-011902</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/416203/teclado-gamer-rise-mode-g1-full-rgb-rainbow-usb-branco-rm-tg-01-fw_1683740597_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/585201/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-preto-920-011902_1718881644_m.jpg</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 66,66</t>
+          <t>R$ 1.221,04</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 30,99</t>
+          <t>R$ 1.099,90</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -697,27 +697,27 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Gamer Redragon Lakshmi Lunar White, Rainbow, Switch Blue, Layout 60%, ABNT2, Branco - K606W-R (PT-BLUE)</t>
+          <t>Teclado Gamer Logitech G PRO X TKL RAPID, Switches Magnético-analógicos, Modo Rapid Trigger, Layout US, Branco - 920-013132</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/285912/teclado-mecanico-gamer-redragon-lakshmi-lunar-white-rainbow-switch-blue-layout-60-abnt2-branco-k606w-r-pt-blue-_1639410278_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/703013/teclado-gamer-logitech-g-pro-x-tkl-rapid-switches-magnetico-analogicos-modo-rapid-trigger-layout-us-branco-920-013132_1740581812_m.jpg</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 211,75</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 159,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -729,27 +729,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Gamer Redragon Kumara, Anti-Ghosting, LED Vermelho, Switch Outemu Red, ABNT2, Preto - K552-2 (PT-RED)</t>
+          <t>Teclado Gamer Semi Mecânico Rise Mode G1 Full, USB, Branco - RM-TG-01-FW</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/93162/93162_2_1523620408_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/416203/teclado-gamer-rise-mode-g1-full-rgb-rainbow-usb-branco-rm-tg-01-fw_1683740597_m.jpg</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 223,52</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>R$ 159,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -761,27 +761,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Teclado Mecânico Gamer HyperX Alloy MKW100, RGB, Switch Red, Full Size, US, Preto - 4P5E1AA#ABA</t>
+          <t>Teclado Mecânico Gamer Redragon Kumara, Anti-Ghosting, LED Vermelho, Switch Outemu Brown, ABNT2, Preto - K552-2 (PT-BROWN)</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/371586/teclado-mecanico-gamer-hyperx-alloy-mkw100-rgb-switch-red-full-size-us-preto-4p5e1aa-aba_1722882381_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/93163/93163_1_1523620161_m.jpg</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 369,55</t>
+          <t>R$ 270,58</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>R$ 269,99</t>
+          <t>R$ 179,99</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/659446/teclado-com-fio-mecanico-gamer-neologic-precision-pro-polar-60-rgb-hot-swap-61-teclas-switch-red-branco-cabo-tipo-c-proplr-red</t>
+          <t>https://www.kabum.com.br/produto/585203/teclado-sem-fio-mecanico-gamer-logitech-g-pro-x-60-lightspeed-rgb-bluetooth-compativel-com-windows-rosa-magenta-920-011940</t>
         </is>
       </c>
     </row>
@@ -793,27 +793,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mouse Gamer Corsair Ironclaw Wireless, RGB, 10 Botões, 18000DPI, Preto - CH-9317011-NA</t>
+          <t>Mouse Gamer Sem Fio Logitech G PRO X Superlight, Lightspeed, 25000 DPI, 5 Botões, Preto - 910-005879</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/109996/mouse-gamer-corsair-wireless-ironclaw-rgb-bluetooth-10-botoes-18000dpi-ch-9317011_1586368589_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/149989/mouse-sem-fio-gamer-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879_1727272012_m.jpg</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 666,66</t>
+          <t>R$ 943,22</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>R$ 469,99</t>
+          <t>R$ 589,99</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -825,27 +825,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Mouse Gamer Sem Fio Logitech G502 X Plus, RGB, 25600 DPI, 13 Botões, Switch, Preto - 910-006161</t>
+          <t>Mouse Gamer Sem Fio Logitech G705, Coleção Aurora, RGB, Bluetooth, USB, 6 Botões, Branco - 910-006366</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/388058/mouse-gamer-sem-fio-logitech-g502-x-plus-rgb-25600-dpi-13-botoes-switch-preto-910-006161_1665144500_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/388060/mouse-gamer-sem-fio-logitech-g705-rgb-bluetooth-usb-6-botoes-branco-910-006366_1664988540_m.jpg</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 1.294,11</t>
+          <t>R$ 613,62</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>R$ 899,99</t>
+          <t>R$ 439,99</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -857,27 +857,27 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Mouse Gamer Corsair M65 Ultra, RGB LED, 26000 DPI, 8 Botões, Optical, Preto - CH-9309411-NA2</t>
+          <t>Mouse Gamer Logitech G502 X, RGB, 25600 DPI, 13 Botões, Switch Híbrido, Branco - 910-006145</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/593795/corsair-m65-rgb-ultra-gaming-mouse-backlit-rgb-led-optical-silver-alu-black-ch-9309411-na2_1729765851_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/388055/mouse-gamer-logitech-g502-x-rgb-25600-dpi-13-botoes-switch-hibrido-branco-910-006145_1665068263_m.jpg</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 711,10</t>
+          <t>R$ 557,88</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>R$ 334,99</t>
+          <t>R$ 429,99</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -889,27 +889,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Mouse Gamer Sem Fio Logitech G703 LIGHTSPEED RGB LIGHTSYNC, 6 Botões Programáveis, HERO 25K, Recarregável, Compatível POWERPLAY - 910-005639</t>
+          <t>Mouse Gamer Sem Fio Logitech G PRO 2 com Lightspeed, RGB Lightsync, Ambidestro, 4 Botões Programáveis, DPI de 32K, Rosa Magenta - 910-007308</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/102651/mouse-gamer-sem-fio-logitech-g703-lightspeed-rgb-lightsync-6-botoes-programaveis-hero-25k-recarregavel-compativel-powerplay-910-005639_1644413882_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/652885/mouse-gamer-sem-fio-logitech-g-pro-2-com-lightspeed-rgb-lightsync-ambidestro-4-botoes-programaveis-dpi-de-32k-rosa-magenta-910-007308_1731094947_m.jpg</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 554,73</t>
+          <t>R$ 777,77</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R$ 429,99</t>
+          <t>R$ 639,99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -921,27 +921,27 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mouse Gamer sem fio Logitech G309 LIGHTSPEED com Switches LIGHTFORCE, Sensor HERO 25K, 6 botões programáveis, Preto - 910-007198</t>
+          <t>Mouse Gamer Sem Fio Logitech G305 Lightspeed, 12.000 DPI, 6 Botões Programáveis, Branco - 910-005290</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/632650/mouse-gamer-sem-fio-logitech-g309-lightspeed-com-switches-lightforce-sensor-hero-25k-6-botoes-programaveis-preto-910-007198_1725913328_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/269638/mouse-gamer-sem-fio-logitech-g305-lightspeed-12-000-dpi-6-botoes-programaveis-branco-910-005290_1637260713_m.jpg</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R$ 623,52</t>
+          <t>R$ 305,87</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>R$ 339,99</t>
+          <t>R$ 233,99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -953,27 +953,27 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Mouse Gamer sem fio Logitech G309 LIGHTSPEED com Switches LIGHTFORCE, Sensor HERO 25K, 6 botões programáveis, Branco - 910-007206</t>
+          <t>Mouse Gamer Trust GXT 960 Graphin RGB, 10.000DPI, 6 Botões, Ultra Leve, Preto - 23758</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/632651/mouse-gamer-sem-fio-logitech-g309-lightspeed-com-switches-lightforce-sensor-hero-25k-6-botoes-programaveis-branco-910-007206_1725913988_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/133479/mouse-gamer-trust-gxt-960-graphin-rgb-10-000dpi-6-botoes-ultra-leve-preto-23758_1607622944_m.jpg</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R$ 623,52</t>
+          <t>R$ 203,17</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>R$ 349,99</t>
+          <t>R$ 164,99</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -985,27 +985,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mouse Gamer Sem Fio Corsair Katar PRO Wireless, RGB, 10000DPI, 6 Botões, Preto - CH-931C011-NA</t>
+          <t>Mouse Gamer Dazz Deathstroke Com Fio, RGB, 10000 DPI, 7 botões - 62000035</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/131190/mouse-gamer-corsair-katar-pro-wireless-rgb-6-botoes-10000dpi-preto-ch-931c011-na_1605117656_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/198650/Mouse-Gamer-Dazz-Deathstroke-Com-Fio-RGB-10000-DPI-7-bot-es-62000035_1730141928_m.jpg</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 374,99</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 229,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -1017,27 +1017,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Mouse Gamer Redragon Cobra, Chroma RGB, 10000DPI, 7 Botões, Preto - M711 V2</t>
+          <t>Mouse Gamer Sem Fio Logitech G305 LIGHTSPEED, 12000 DPI, 6 Botões, Preto - 910-005281</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/94555/mouse-gamer-redragon-cobra-chroma-rgb-12400dpi-7-botoes-preto-m711-v2_1656018617_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/97092/97092_3_1528977678_m.jpg</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R$ 152,93</t>
+          <t>R$ 294,11</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>R$ 93,99</t>
+          <t>R$ 244,99</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -1049,27 +1049,27 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Mouse Gamer Redragon Predator, Chroma RGB, 8000DPI, 9 Botões, Preto - M612</t>
+          <t>Mouse Gamer Redragon Cobra, Chroma RGB, 10000DPI, 7 Botões, Preto - M711 V2</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/133482/mouse-gamer-redragon-predator-rgb-m612_1608738736_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/94555/mouse-gamer-redragon-cobra-chroma-rgb-10000dpi-7-botoes-preto-m711-v2_1742821619_m.jpg</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>R$ 141,16</t>
+          <t>R$ 152,93</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>R$ 79,99</t>
+          <t>R$ 89,99</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -1081,27 +1081,27 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Mouse Gamer Sem Fio Redragon Storm Pro, RGB, 16000 DPI, 8 Botões, Wireless, Preto - M808-KS</t>
+          <t>Mouse Gamer Redragon Predator, Chroma RGB, 8000DPI, 9 Botões, Preto - M612</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/523248/mouse-gamer-sem-fio-redragon-storm-pro-rgb-16000-dpi-8-botoes-wireless-preto-m808-ks_1717675137_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/133482/mouse-gamer-redragon-predator-rgb-m612_1608738736_m.jpg</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>R$ 276,46</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>R$ 168,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/109996/mouse-gamer-corsair-ironclaw-wireless-rgb-10-botoes-18000dpi-preto-ch-9317011-na</t>
+          <t>https://www.kabum.com.br/produto/149989/mouse-gamer-sem-fio-logitech-g-pro-x-superlight-lightspeed-25000-dpi-5-botoes-preto-910-005879</t>
         </is>
       </c>
     </row>
@@ -1113,27 +1113,27 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Headset Gamer Logitech G335, 3.5mm para PC/PlayStation/Xbox/Switch/Mobile, Driver 40mm, Arco Ajustável, Verde - 981-001023</t>
+          <t>Headset Gamer Com Fio Quantum 100m2 Jbl Com Mic, Preto - 28913835</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023_1627326460_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835_1737384092_m.jpg</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>R$ 421,04</t>
+          <t>R$ 277,77</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>R$ 349,99</t>
+          <t>R$ 159,99</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1145,27 +1145,27 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Headset Gamer Sem Fio Logitech G Astro A50 X LIGHTSPEED + Base Station, Bluetooth, HDMI 2.1 Passthru, para Xbox e PS, Preto- 939-002126</t>
+          <t>Headset Gamer Over-ear Beyerdynamic Mmx 150, Usb, PC, XBOX, Ps4, Ps5 - Grey</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/579717/headset-gamer-sem-fio-logitech-g-astro-a50-x-lightspeed-base-station-bluetooth-para-xbox-e-ps-preto-939-002126_1715279047_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/649794/Headset-Gamer-Over-ear-Beyerdynamic-Mmx-150-Usb-Pc-Xbox-Ps4-Ps5-Grey_1729258591_m.jpg</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>R$ 3.058,81</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>R$ 1.989,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1177,27 +1177,27 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Headset Gamer Sem Fio Logitech G435, Lightspeed e Bluetooth, Dolby Atmos, USB, PC, PS4, PS5, Mobile, Drivers 40mm, Branco - 981-001073</t>
+          <t>Headset Gamer Force One Titan, RGB, 7.1 Surround, 50mm, USB, PC e Playstation, Branco</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/263078/headset-gamer-sem-fio-logitech-g435-lightspeed-e-bluetooth-dolby-atmos-usb-pc-ps4-ps5-mobile-drivers-40mm-branco-981-001073_1636555971_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/468215/Headset-Gamer-Force-One-Titan-RGB-7-1-Surround-50mm-USB-PC-e-Playstation-Branco_1686068899_m.jpg</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>R$ 741,16</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>R$ 559,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1209,27 +1209,27 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Headset Gamer Logitech G335, 3.5mm para PC/PlayStation/Xbox/Switch/Mobile, Driver 40mm, Arco Ajustável, Branco - 981-001017</t>
+          <t>Headset Gamer Logitech G Astro A10, Drivers 40mm, P3, PS e PC, Branco - 939-002063</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/181877/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-branco-981-001017_1627325453_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/404401/headset-gamer-astro-a10-drivers-40mm-p3-ps-e-pc-branco-939-002063_1670871092_m.jpg</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>R$ 523,97</t>
+          <t>R$ 555,54</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>R$ 348,90</t>
+          <t>R$ 449,99</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1241,27 +1241,27 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Headset Gamer Sem Fio Logitech G435, Lightspeed e Bluetooth, Dolby Atmos, USB, PC, PS4, PS5, Mobile, Drivers 40mm, Azul - 981-001061</t>
+          <t>Headset Gamer Sem Fio Logitech G Pro X 2 Lightspeed, Driver 50mm, Bluetooth, USB e 3.5mm, para PC, Playstation e Switch, Preto - 981-001262</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/263079/headset-gamer-sem-fio-logitech-g435-lightspeed-e-bluetooth-dolby-atmos-usb-pc-ps4-ps5-mobile-drivers-40mm-azul-981-001061_1636557309_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/495541/headset-gamer-sem-fio-logitech-g-pro-x-2-lightspeed-bluetooth-usb-e-3-5mm-para-pc-playstation-e-switch-preto-981-001262_1696601355_m.jpg</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>R$ 733,58</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>R$ 459,90</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1273,27 +1273,27 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Headset Gamer Havit, Drivers 53mm, Microfone Plugável, P2, PC, PS4, XBOX ONE, Preto - HV-H2002D</t>
+          <t>Headset JBL Quantum 910 Gamer Wireless RGB Hi-Res, PS5, PS4, Nintendo Switch - JBLQ910WLBLK</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/102770/headset-gamer-havit-drivers-53mm-hv-h2002d_headset-gamer-havit-drivers-53mm-hv-h2002d_1564056874_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/468474/headset-jbl-quantum-910-gamer-wireless-rgb-hi-res-ps5-ps4-nintendo-switch-jblq910wlblk_1688495852_m.jpg</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>R$ 258,81</t>
+          <t>R$ 1.682,34</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>R$ 159,90</t>
+          <t>R$ 1.299,99</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1305,27 +1305,27 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Headset Gamer HyperX Cloud Stinger 2, Drivers 50mm, P3, Preto - 519T1AA</t>
+          <t>Headset Gamer Sem Fio Astro A50 + Base Station Gen 4 com Áudio Dolby Atmos para Xbox Series, Xbox One, PC, Mac - Preto - 939-001681</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/461160/headset-gamer-hyperx-cloud-stinger-2-drivers-50mm-preto-519t1aa_1689972862_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/102653/headset-sem-fio-gamer-astro-a50-base-station-gen4-xbox-one-pc-dolby-audio-v2_headset-sem-fio-gamer-astro-a50-base-station-gen4-xbox-one-pc-dolby-audio-v2_1563560943_m.jpg</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>R$ 361,16</t>
+          <t>R$ 2.209,47</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>R$ 232,99</t>
+          <t>R$ 1.799,99</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1337,27 +1337,27 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Headset Gamer Redragon Lamia 2, RGB, 7.1, 40mm, Suporte Incluso - H320RGB-1</t>
+          <t>Headset Gamer Sem Fio Logitech G733 7.1 Dolby Surround RGB LIGHTSYNC, Blue VOICE para PC e PlayStation, Preto - 981-000863</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/115413/headset-gamer-redragon-lamia-rgb-drivers-40mm-h320rgb-1-_1595016854_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/120487/headset-gamer-sem-fio-logitech-g733-rgb-lightsync-7-1-dolby-surround-com-blue-voice-preto-981-000863_1612874214_m.jpg</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>R$ 188,22</t>
+          <t>R$ 1.304,34</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>R$ 155,99</t>
+          <t>R$ 848,99</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1369,27 +1369,27 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Headset Gamer Redragon Zeus X RGB, Surround 7.1, Driver de 53mm, USB, Microfone com Redução de Ruído, Branco com Rosê - H510WR-RGB</t>
+          <t>Headset Gamer Redragon Zeus X, Chroma Mk.II, RGB, Som Surround 7.1, Drivers 53mm, USB, Preto e Vermelho - H510-RGB</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/335825/headset-gamer-redragon-zeus-x-rgb-surround-7-1-driver-de-53mm-usb-microfone-com-reducao-de-ruido-branco-com-rose-h510wr-rgb_1652451567_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/227818/headset-gamer-redragon-zeus-chroma-mk-ii-rgb-surround-7-1-usb-drivers-53mm-preto-vermelho-h510-rgb_1631555309_m.jpg</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>R$ 335,28</t>
+          <t>R$ 423,52</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>R$ 239,99</t>
+          <t>R$ 349,99</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1401,27 +1401,27 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Headset Gamer Redragon Zeus X, Chroma Mk.II, RGB, Som Surround 7.1, Drivers 53mm, USB, Preto e Vermelho - H510-RGB</t>
+          <t>Headset Gamer Sem Fio Havit Fuxi H3, 7.1 surround, Driver 40mm, Bluetooth e USB, Preto - Fuxi-H3 Black</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/227818/headset-gamer-redragon-zeus-chroma-mk-ii-rgb-surround-7-1-usb-drivers-53mm-preto-vermelho-h510-rgb_1631555309_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/519934/headset-gamer-sem-fio-havit-fuxi-h3-7-1-surround-driver-40mm-bluetooth-e-usb-preto-fuxi-h3-black_1706888697_m.jpg</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>R$ 388,22</t>
+          <t>R$ 292,62</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>R$ 312,99</t>
+          <t>R$ 199,99</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/181878/headset-gamer-logitech-g335-3-5mm-para-pc-playstation-xbox-switch-mobile-driver-40mm-arco-ajustavel-verde-981-001023</t>
+          <t>https://www.kabum.com.br/produto/670662/headset-gamer-com-fio-quantum-100m2-jbl-com-mic-preto-28913835</t>
         </is>
       </c>
     </row>
@@ -1433,27 +1433,27 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Monitor Gamer LG UltraGear 27" IPS Full HD, 180Hz, 1ms GTG, DisplayPort e HDMI, G-Sync, FreeSync, HDR10, sRGB 99%, Preto - 27GS60F-B</t>
+          <t>Monitor Gamer Curvo AOC Legend 27", 240Hz, Full HD, 0.5ms, DisplayPort e HDMI, FreeSync Premium, 120% sRGB - C27G2ZE</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b_1725043961_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/229561/monitor-gamer-aoc-legend-27-led-curvo-240-hz-full-hd-0-5ms-freesync-premium-120-srgb-hdmi-displayport-c27g2ze_1632937089_m.jpg</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>R$ 1.388,88</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>R$ 1.099,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1475,17 +1475,17 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>R$ 777,77</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>R$ 649,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1497,12 +1497,12 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Monitor Gamer LG UltraGear 24" Full HD, IPS, 180Hz, 1ms GTG, DisplayPort e HDMI, NVIDIA G-SYNC , AMD FreeSync, HDR10, sRGB 99% - 24GS60F-B</t>
+          <t>Monitor Gamer AOC 24" FHD, IPS, 180Hz, 0,5ms, HDMI e DP, W-LED, Antireflexo, Ajuste de Altura, Preto - 24G4/P</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/614879/monitor-gamer-lg-ultragear-24-full-hd-ips-180hz-1ms-displayport-e-hdmi-nvidia-g-sync-amd-freesync-hdr10-srgb-99-24gs60f-b_1722881105_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/659038/monitor-gamer-aoc-24-fhd-ips-180hz-0-5ms-hdmi-e-dp-w-led-antireflexo-ajuste-de-altura-preto-24g4-p_1733834296_m.jpg</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1512,12 +1512,12 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>R$ 1.017,82</t>
+          <t>R$ 899,99</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1529,12 +1529,12 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Monitor Gamer LG 21.5", 75Hz, Full HD, HDMI, FreeSync - 22MP410-B</t>
+          <t>Monitor Gamer Samsung Odyssey G40 27" FHD, 240Hz, 1ms, Ajuste De Altura, Hdmi, Dp, Gsync, Freesync, Preto - Ls27bg400elxzd</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/397845/monitor-gamer-lg-21-5-75hz-full-hd-hdmi-freesync-22mp410-b_1733861519_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/374599/Monitor-Gamer-Samsung-Odyssey-G40-27-FHD-Tela-Plana-240Hz-1Ms-HDMI-Freesync-Premium-G-Sync-Preto_1731182743_m.jpg</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1549,7 +1549,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1561,27 +1561,27 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Monitor Gamer Curvo LG UltraGear LG 34", UltraWide, 160Hz, WQHD, 1ms, DisplayPort e HDMI, AMD FreeSync Premium, HDR10, 99% sRGB - 34GP63A-B</t>
+          <t>Monitor Gamer Samsung Odyssey G40 25" FHD, 240Hz, 1ms, Ajuste De Altura, Hdmi, Dp, Gsync, Freesync, Preto</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/472908/monitor-gamer-lg-ultragear-lg-34-curvo-led-wqhd-ultrawide-160hz-1ms-displayport-e-hdmi-amd-freesync-premium-hdr10-99-srgb-34gp63a-b_1717591886_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/374598/Monitor-Gamer-Samsung-Odyssey-G40-25-FHD-Tela-Plana-240Hz-1Ms-HDMI-FreeSync-Premium-G-Sync_1731181442_m.jpg</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>R$ 2.999,99</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>R$ 2.199,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1593,27 +1593,27 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Monitor Gamer Curvo Concórdia 27'', 100Hz, Led FULL HD, HDMI, VGA - Cz270f</t>
+          <t>Monitor Gamer Samsung 22" FHD,100 Hz, HDMI, VGA,Preto, S3</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/504136/Monitor-Gamer-Curvo-Conc-rdia-27-100Hz-Led-FULL-HD-HDMI-VGA-Cz270f_1730123291_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/723085/medium/Monitor-Gamer-Samsung-22-FHD-100-Hz-HDMI-VGA-Preto-S3_1744121490.jpg</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>R$ 883,00</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>R$ 679,00</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1625,12 +1625,12 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Monitor Gamer LG 27 Full HD, IPS, HDMI e VESA, FreeSync, Ajuste de Ângulo, Bordas Finas - 27MP400-B</t>
+          <t>Monitor Gamer Samsung T350, 75Hz, 5Ms, HDMI, 22" FULL HD Tela Plana, FreeSync, Game Mode</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/323895/monitor-gamer-lg-27-full-hd-ips-hdmi-e-vesa-freesync-ajuste-de-angulo-bordas-finas-27mp400-b_1721412719_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/254368/medium/Monitor-Gamer-Samsung-T350-75Hz-5Ms-HDMI-22-FULL-HD-Tela-Plana-FreeSync-Game-Mode_1740519117.jpg</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1645,7 +1645,7 @@
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1657,27 +1657,27 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Monitor Gamer Aoc 27" Full HD, 165Hz, 1Ms, Displayport, HDMI E VGA, Ajuste De Altura - 27g2s/bk</t>
+          <t>Monitor Gamer Samsung 24" FHD,100 Hz, HDMI, VGA,Preto, S3</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/586255/monitor-gamer-aoc-27-165hz-full-hd-1ms-displayport-hdmi-e-vga-ajuste-de-altura-27g2s-bk_1731515821_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/724790/medium/Monitor-Gamer-Samsung-24-FHD-100-Hz-HDMI-VGA-Preto-S3_1744120875.jpg</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>R$ 979,00</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>R$ 881,10</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1689,27 +1689,27 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Monitor Gamer Curvo KBM! GAMING MG210 23.6", 180Hz, Full HD, 1ms, DisplayPort e HDMI, Adaptive Sync, Ajuste de Ângulo - KGMG21023PT</t>
+          <t>Monitor Gamer LG UltraGear 27" FHD, IPS, 180Hz, 1ms GTG, HDR10, DisplayPort e HDMI, G-Sync, FreeSync, Preto - 27GS60F-B</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/471916/monitor-gamer-curvo-kbm-gaming-mg210-23-6-180hz-full-hd-1ms-displayport-e-hdmi-adaptive-sync-ajuste-de-angulo-kgmg21023pt_1722535322_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b_1725043961_m.jpg</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>R$ 888,88</t>
+          <t>R$ 1.555,54</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>R$ 699,99</t>
+          <t>R$ 999,99</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1721,27 +1721,27 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Monitor Gamer LG UltraGear 27", 144Hz, Full HD, 1ms, IPS, DisplayPort e HDMI, HDR 10, 99% sRGB, FreeSync Premium, VESA - 27GN65R</t>
+          <t>Monitor Gamer Concórdia 23,8 LED Full HD, 165Hz, 1ms, HDMI/DisplayPort, FreeSync, Preto e Prata - R200s</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/444038/monitor-gamer-lg-ultragear-27-full-hd-144hz-1ms-ips-hdmi-e-displayport-hdr-10-99-srgb-freesync-premium-vesa-27gn65r_1712149543_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/365026/monitor-gamer-concordia-23-8-led-full-hd-165hz-1ms-hdmi-displayport-freesync-preto-e-prata-r200s_1658262184_m.jpg</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>R$ 1.366,66</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>R$ 1.099,99</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>https://www.kabum.com.br/produto/620992/monitor-gamer-lg-ultragear-27-ips-full-hd-180hz-1ms-gtg-displayport-e-hdmi-g-sync-freesync-hdr10-srgb-99-preto-27gs60f-b</t>
+          <t>https://www.kabum.com.br/produto/229561/monitor-gamer-curvo-aoc-legend-27-240hz-full-hd-0-5ms-displayport-e-hdmi-freesync-premium-120-srgb-c27g2ze</t>
         </is>
       </c>
     </row>
@@ -1763,12 +1763,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Sem informações anteriores</t>
+          <t>R$ 752,58</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Sem informações recentes</t>
+          <t>R$ 589,90</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -1785,22 +1785,22 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Branco, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600BR</t>
+          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Preta, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600PT</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/471927/cadeira-gamer-kbm-gaming-cg600-branco-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600br_1700660778_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/471925/cadeira-gamer-kbm-gaming-tempest-cg600-preta-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600pt_1728407130_m.jpg</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>R$ 1.222,11</t>
+          <t>R$ 1.314,10</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>R$ 899,90</t>
+          <t>R$ 919,90</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -1817,22 +1817,22 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Preta, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600PT</t>
+          <t>Cadeira Gamer KBM! GAMING CG200, Preto e Branco - Pistão Classe 3, Almofadas cabeça e lombar - KGCG200PTBR</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/471925/cadeira-gamer-kbm-gaming-tempest-cg600-preta-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600pt_1728407130_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/477693/cadeira-gamer-kbm-gaming-cg200-preto-e-branco-pistao-classe-3-almofadas-cabeca-e-lombar-kgcg200ptbr_1707392209_m.jpg</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>R$ 1.357,90</t>
+          <t>R$ 860,11</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>R$ 899,90</t>
+          <t>R$ 589,90</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
@@ -1849,12 +1849,12 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Cadeira Gamer Mymax Mx5, Até 150KG, Almofadas, Ergonômica, Couro Sintético - Preto e Branco</t>
+          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Branco, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600BR</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/265788/Cadeira-Gamer-Mymax-Mx5-At-150KG-Almofadas-Ergon-mica-Couro-Sint-tico-Preto-e-Branco_1726250397_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/471927/cadeira-gamer-kbm-gaming-cg600-branco-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600br_1700660778_m.jpg</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1881,22 +1881,22 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Cadeira Gamer Vermelha Prizi - Jx-1039r</t>
+          <t>Cadeira Gamer KBM! GAMING Tempest CG500 Preta Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG500PT</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/309110/Cadeira-Gamer-Vermelha-Prizi-Jx-1039r_1721996455_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/471926/cadeira-gamer-kbm-gaming-cg500-preta-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg500pt_1700827595_m.jpg</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>Sem informações anteriores</t>
+          <t>R$ 1.128,93</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>Sem informações recentes</t>
+          <t>R$ 799,90</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
@@ -1913,22 +1913,22 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Cinza Claro, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600CZ</t>
+          <t>Cadeira Gamer Mymax Mx5, Até 150Kg, Giratória e Ergonômica - Preto</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/471928/cadeira-gamer-kbm-gaming-cg600-cinza-claro-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600cz_1700662493_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/265789/medium/Cadeira-Gamer-Mymax-Mx5-At-150Kg-Girat-ria-e-Ergon-mica-Preto_1743782433.jpg</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>R$ 1.222,11</t>
+          <t>Sem informações anteriores</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>R$ 899,90</t>
+          <t>Sem informações recentes</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -1945,22 +1945,22 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Cadeira Gamer Prizi Canvas, Até 120Kg, Com Almofadas, Branca</t>
+          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Preta e Vermelho, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600PTVM</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/322242/Cadeira-Gamer-Prizi-Canvas-At-120Kg-Com-Almofadas-Branca_1726079148_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/471929/cadeira-gamer-kbm-gaming-cg600-preta-e-vermelho-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600ptvm_1700678542_m.jpg</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Sem informações anteriores</t>
+          <t>R$ 1.182,69</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Sem informações recentes</t>
+          <t>R$ 899,90</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
@@ -1977,22 +1977,22 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Cadeira Gamer KBM! GAMING Tempest CG500 Preta Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG500PT</t>
+          <t>Cadeira Gamer KBM! GAMING Tempest CG600, Cinza Claro, Com Almofadas, Descanso Para Pernas Retrátil, Reclinável - KGCG600CZ</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/471926/cadeira-gamer-kbm-gaming-cg500-preta-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg500pt_1700827595_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/471928/cadeira-gamer-kbm-gaming-cg600-cinza-claro-com-almofadas-descanso-para-pernas-retratil-reclinavel-kgcg600cz_1700662493_m.jpg</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>R$ 1.166,56</t>
+          <t>R$ 1.021,39</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>R$ 859,90</t>
+          <t>R$ 899,90</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -2009,12 +2009,12 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Cadeira Gamer Falcon, Até 150Kg - Edge Preta</t>
+          <t>Cadeira Gamer Prizi Canvas, Até 120Kg, Com Almofadas, Preta</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/586916/Cadeira-Gamer-Falcon-At-150Kg-Edge-Preta_1722346310_m.jpg</t>
+          <t>https://images.kabum.com.br/produtos/fotos/sync_mirakl/320744/Cadeira-Gamer-Prizi-Canvas-At-120Kg-Com-Almofadas-Preta_1723123517_m.jpg</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2051,12 +2051,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>R$ 777,67</t>
+          <t>R$ 752,58</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>R$ 559,90</t>
+          <t>R$ 589,90</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">

</xml_diff>